<commit_message>
Feat: "dialogue 시스템 구현"
</commit_message>
<xml_diff>
--- a/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/SelectDB.xlsx
+++ b/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/SelectDB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B7931-A0C9-41E1-A4E7-F792EAC72871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AEF9D-326D-4E1F-80E7-2CFB32F49B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,15 +61,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"8"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"-7.8164"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"2.4856"</t>
+    <t>선택지3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처음으로 돌아가요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탈출해요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -479,28 +479,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" s="1">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>